<commit_message>
added program in table format
</commit_message>
<xml_diff>
--- a/content/en/program/CASCONProgramTable.xlsx
+++ b/content/en/program/CASCONProgramTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josenelsonamaral/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josenelsonamaral/service/conferences/CASCON24/webpage/CASCON2024/content/en/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3218259-C6CA-7C45-B838-45ECDF4F132A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472C324E-569D-184A-8A77-14D9E0B19A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="780" windowWidth="27240" windowHeight="16440" xr2:uid="{7DC0458B-76C0-C743-8050-45CEC12FF2F3}"/>
+    <workbookView xWindow="8880" yWindow="780" windowWidth="27240" windowHeight="16440" xr2:uid="{7DC0458B-76C0-C743-8050-45CEC12FF2F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>Breakfast</t>
   </si>
@@ -87,10 +87,6 @@
   <si>
     <t>CDP
 Room C2</t>
-  </si>
-  <si>
-    <t>AI@Work
-Room D2</t>
   </si>
   <si>
     <t>Tuesday, November 12</t>
@@ -156,6 +152,10 @@
   </si>
   <si>
     <t>Conference Banquet</t>
+  </si>
+  <si>
+    <t>AI@Work
+Room 344</t>
   </si>
 </sst>
 </file>
@@ -348,149 +348,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -806,71 +810,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF72406-836C-1D48-B2CA-0E5E52338AF8}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="32"/>
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="47"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="33"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="34">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="30">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="23">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="9" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="5"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="30"/>
     </row>
-    <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="34">
+    <row r="3" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="26">
         <v>0.35416666666666669</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -879,60 +885,62 @@
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="23">
         <v>0.35416666666666669</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="44"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="43"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="34">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="26">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="30">
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="23">
         <v>0.39583333333333331</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="13" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="6"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="41"/>
     </row>
-    <row r="5" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="34">
+    <row r="5" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="26">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -941,76 +949,78 @@
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="23">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="49"/>
+      <c r="M5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="N5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>22</v>
+      <c r="P5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="34">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="26">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="30">
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="23">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="13" t="s">
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="6"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="41"/>
     </row>
-    <row r="7" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="34">
+    <row r="7" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="26">
         <v>0.5625</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1019,199 +1029,209 @@
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="23">
         <v>0.5625</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="15" t="s">
+      <c r="K7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="P7" s="19" t="s">
-        <v>23</v>
+      <c r="O7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="34">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="26">
         <v>0.625</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="30">
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="23">
         <v>0.625</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="13" t="s">
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="6"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="41"/>
     </row>
-    <row r="9" spans="1:16" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+    <row r="9" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="N9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="P9" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="36" t="s">
+      <c r="G11" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="G1:L1"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G11:L11"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="L6:P6"/>
-    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="M4:Q4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="G2:K2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K7" r:id="rId1" display="mailto:https://github.com/ICCSSE/CASCON2024/blob/main/content/en/workshops/AI%40Work.pdf" xr:uid="{4B833420-C683-B944-BAE9-635EB9494485}"/>
-    <hyperlink ref="K5" r:id="rId2" display="https://users.encs.concordia.ca/~abdelw/oxai2024/" xr:uid="{FD0F26E3-265C-CD43-BE38-B7242A72D16F}"/>
-    <hyperlink ref="K9" r:id="rId3" display="mailto:https://github.com/ICCSSE/CASCON2024/blob/main/content/en/workshops/AI%40Work.pdf" xr:uid="{CCC28448-E19C-0B4A-B3F2-1F568AF8C5CC}"/>
-    <hyperlink ref="J5" r:id="rId4" display="mailto:https://cdp-workshop.github.io/CDP/" xr:uid="{921351A4-4D98-1949-8A7B-646BF94841E3}"/>
-    <hyperlink ref="J7" r:id="rId5" display="mailto:https://cdp-workshop.github.io/CDP/" xr:uid="{4316EBAD-7B91-0048-BD4C-65E1846D6281}"/>
-    <hyperlink ref="J9" r:id="rId6" display="mailto:https://cdp-workshop.github.io/CDP/" xr:uid="{4CC758FD-A387-7742-83C5-43997787AAE9}"/>
-    <hyperlink ref="I5" r:id="rId7" location="iM-PACT" display="mailto:https://cascon.ca/workshops/ - iM-PACT" xr:uid="{46CA5009-AA88-1346-A397-4075A864F20E}"/>
-    <hyperlink ref="I7" r:id="rId8" location="DITA" display="mailto:https://cascon.ca/workshops/ - DITA" xr:uid="{CE5ADC8D-0E5B-F644-B65F-31C8D818531A}"/>
-    <hyperlink ref="I9" r:id="rId9" location="DITA" display="mailto:https://cascon.ca/workshops/ - DITA" xr:uid="{517F551F-70E3-3740-A95E-35A8FE8E73CA}"/>
-    <hyperlink ref="E3" r:id="rId10" display="https://sites.google.com/view/cypress2024/" xr:uid="{41B2562C-C3F3-0A49-A248-6CF17B2F3564}"/>
-    <hyperlink ref="N7" r:id="rId11" location="AgileKip" display="https://cascon.ca/workshops/ - AgileKip" xr:uid="{C3CD8432-1733-CB47-8113-803842B82D1E}"/>
-    <hyperlink ref="O5" r:id="rId12" location="ClientZero" display="https://cascon.ca/workshops/ - ClientZero" xr:uid="{3457E14B-63A5-024C-9D4F-C946B0BAE98C}"/>
-    <hyperlink ref="L5" r:id="rId13" location="ML4DM" display="https://cascon.ca/workshops/ - ML4DM" xr:uid="{E1A4D481-EF17-1C48-B078-1D238441B226}"/>
-    <hyperlink ref="N5" r:id="rId14" location="SENGEC" display="https://cascon.ca/workshops/ - SENGEC" xr:uid="{8BCF09AF-500B-4D4A-9B1C-56D24829261A}"/>
-    <hyperlink ref="P5" r:id="rId15" display="https://github.com/ZeruiW/CASCON24_Tutorial-Workshop_XAI/blob/main/Develop Explainable AI Services on Cloud Computing and Open Source Models.md" xr:uid="{0E75BFF7-3191-7349-8176-7A29285C00D1}"/>
-    <hyperlink ref="O7" r:id="rId16" location="PACOLA" display="https://cascon.ca/workshops/ - PACOLA" xr:uid="{85DC61E8-ECEB-1347-AE30-535711BB3388}"/>
-    <hyperlink ref="P7" r:id="rId17" location="NatLang" display="https://cascon.ca/workshops/ - NatLang" xr:uid="{94E8C3BE-E863-9740-BDDF-77DD9957203B}"/>
-    <hyperlink ref="G3:K3" r:id="rId18" display="https://cascon.ca/keynotes/" xr:uid="{ABC01048-2211-1348-858B-56807C76450F}"/>
-    <hyperlink ref="L3:P3" r:id="rId19" display="https://cascon.ca/keynotes/" xr:uid="{F636CE58-D2FA-784A-A1BE-AEC64C394F38}"/>
-    <hyperlink ref="L7" r:id="rId20" location="ML4DM" display="https://cascon.ca/workshops/ - ML4DM" xr:uid="{16E10E96-BF1E-9C4A-9F1E-24267FB1F862}"/>
-    <hyperlink ref="L9" r:id="rId21" location="ML4DM" display="https://cascon.ca/workshops/ - ML4DM" xr:uid="{79EEAD2A-EF00-2741-87B1-34BC7EE08DCD}"/>
-    <hyperlink ref="O9" r:id="rId22" location="PACOLA" display="https://cascon.ca/workshops/ - PACOLA" xr:uid="{AD0D8FF1-4DF1-014B-A88D-B02080B83048}"/>
-    <hyperlink ref="N9" r:id="rId23" location="AgileKip" display="https://cascon.ca/workshops/ - AgileKip" xr:uid="{6C6BB10E-FEE3-134A-B797-514AA6A63D4B}"/>
-    <hyperlink ref="E7" r:id="rId24" location="CASCON1" display="https://cascon.ca/program/ - CASCON1" xr:uid="{2DE4E056-2864-084A-A7D1-080A0D090EF4}"/>
-    <hyperlink ref="E9" r:id="rId25" location="CASCON2" display="https://cascon.ca/program/ - CASCON2" xr:uid="{AEF291A1-B334-9149-ADB6-A08474B1EE6E}"/>
-    <hyperlink ref="H5" r:id="rId26" location="CASCON3" display="https://cascon.ca/program/ - CASCON3" xr:uid="{4F746670-2124-0243-A890-EFFB2DDAB8C2}"/>
-    <hyperlink ref="H7" r:id="rId27" location="CASCON4" display="https://cascon.ca/program/ - CASCON4" xr:uid="{86AD4F9A-9827-9249-915A-DC0C0A9E74C8}"/>
-    <hyperlink ref="H9" r:id="rId28" location="CASCON5" display="https://cascon.ca/program/ - CASCON5" xr:uid="{35B56934-3EE5-3047-8511-B40F7A01AFAE}"/>
-    <hyperlink ref="M5" r:id="rId29" location="CASCON6" display="https://cascon.ca/program/ - CASCON6" xr:uid="{637AB7B5-AE20-E24E-95EC-9FCA93947DB0}"/>
-    <hyperlink ref="M7" r:id="rId30" location="CASCON7" display="https://cascon.ca/program/ - CASCON7" xr:uid="{E8A68215-B911-D14D-BB9A-EA6A152D4829}"/>
-    <hyperlink ref="M9" r:id="rId31" location="CASCON8" display="https://cascon.ca/program/ - CASCON8" xr:uid="{EB0DAB3C-289F-FD4C-A871-C58B0ABBA63C}"/>
-    <hyperlink ref="E5" r:id="rId32" display="https://sites.google.com/view/cypress2024/" xr:uid="{F8B4BFBE-7F83-F14D-8F0D-63AEF530B43F}"/>
-    <hyperlink ref="P9" r:id="rId33" location="NatLang" display="https://cascon.ca/workshops/ - NatLang" xr:uid="{43DF3043-FF6A-A24C-AACE-26632CD05EDF}"/>
-    <hyperlink ref="G11:K11" r:id="rId34" display="CASCON Poster Presentations and Reception" xr:uid="{3AA7171D-8394-0E42-8AE6-6B2708A831E7}"/>
+    <hyperlink ref="L7" r:id="rId1" xr:uid="{4B833420-C683-B944-BAE9-635EB9494485}"/>
+    <hyperlink ref="L9" r:id="rId2" xr:uid="{CCC28448-E19C-0B4A-B3F2-1F568AF8C5CC}"/>
+    <hyperlink ref="J5" r:id="rId3" display="mailto:https://cdp-workshop.github.io/CDP/" xr:uid="{921351A4-4D98-1949-8A7B-646BF94841E3}"/>
+    <hyperlink ref="J7" r:id="rId4" display="mailto:https://cdp-workshop.github.io/CDP/" xr:uid="{4316EBAD-7B91-0048-BD4C-65E1846D6281}"/>
+    <hyperlink ref="J9" r:id="rId5" display="mailto:https://cdp-workshop.github.io/CDP/" xr:uid="{4CC758FD-A387-7742-83C5-43997787AAE9}"/>
+    <hyperlink ref="I5" r:id="rId6" location="iM-PACT" display="mailto:https://cascon.ca/workshops/ - iM-PACT" xr:uid="{46CA5009-AA88-1346-A397-4075A864F20E}"/>
+    <hyperlink ref="I7" r:id="rId7" location="DITA" display="mailto:https://cascon.ca/workshops/ - DITA" xr:uid="{CE5ADC8D-0E5B-F644-B65F-31C8D818531A}"/>
+    <hyperlink ref="I9" r:id="rId8" location="DITA" display="mailto:https://cascon.ca/workshops/ - DITA" xr:uid="{517F551F-70E3-3740-A95E-35A8FE8E73CA}"/>
+    <hyperlink ref="E3" r:id="rId9" display="https://sites.google.com/view/cypress2024/" xr:uid="{41B2562C-C3F3-0A49-A248-6CF17B2F3564}"/>
+    <hyperlink ref="O7" r:id="rId10" location="AgileKip" display="https://cascon.ca/workshops/ - AgileKip" xr:uid="{C3CD8432-1733-CB47-8113-803842B82D1E}"/>
+    <hyperlink ref="P5" r:id="rId11" location="ClientZero" display="https://cascon.ca/workshops/ - ClientZero" xr:uid="{3457E14B-63A5-024C-9D4F-C946B0BAE98C}"/>
+    <hyperlink ref="M5" r:id="rId12" location="ML4DM" display="https://cascon.ca/workshops/ - ML4DM" xr:uid="{E1A4D481-EF17-1C48-B078-1D238441B226}"/>
+    <hyperlink ref="O5" r:id="rId13" location="SENGEC" display="https://cascon.ca/workshops/ - SENGEC" xr:uid="{8BCF09AF-500B-4D4A-9B1C-56D24829261A}"/>
+    <hyperlink ref="Q5" r:id="rId14" display="https://github.com/ZeruiW/CASCON24_Tutorial-Workshop_XAI/blob/main/Develop Explainable AI Services on Cloud Computing and Open Source Models.md" xr:uid="{0E75BFF7-3191-7349-8176-7A29285C00D1}"/>
+    <hyperlink ref="P7" r:id="rId15" location="PACOLA" display="https://cascon.ca/workshops/ - PACOLA" xr:uid="{85DC61E8-ECEB-1347-AE30-535711BB3388}"/>
+    <hyperlink ref="Q7" r:id="rId16" location="NatLang" display="https://cascon.ca/workshops/ - NatLang" xr:uid="{94E8C3BE-E863-9740-BDDF-77DD9957203B}"/>
+    <hyperlink ref="G3:L3" r:id="rId17" display="https://cascon.ca/keynotes/" xr:uid="{ABC01048-2211-1348-858B-56807C76450F}"/>
+    <hyperlink ref="M3:Q3" r:id="rId18" display="https://cascon.ca/keynotes/" xr:uid="{F636CE58-D2FA-784A-A1BE-AEC64C394F38}"/>
+    <hyperlink ref="M7" r:id="rId19" location="ML4DM" display="https://cascon.ca/workshops/ - ML4DM" xr:uid="{16E10E96-BF1E-9C4A-9F1E-24267FB1F862}"/>
+    <hyperlink ref="M9" r:id="rId20" location="ML4DM" display="https://cascon.ca/workshops/ - ML4DM" xr:uid="{79EEAD2A-EF00-2741-87B1-34BC7EE08DCD}"/>
+    <hyperlink ref="P9" r:id="rId21" location="PACOLA" display="https://cascon.ca/workshops/ - PACOLA" xr:uid="{AD0D8FF1-4DF1-014B-A88D-B02080B83048}"/>
+    <hyperlink ref="O9" r:id="rId22" location="AgileKip" display="https://cascon.ca/workshops/ - AgileKip" xr:uid="{6C6BB10E-FEE3-134A-B797-514AA6A63D4B}"/>
+    <hyperlink ref="E7" r:id="rId23" location="CASCON1" display="https://cascon.ca/program/ - CASCON1" xr:uid="{2DE4E056-2864-084A-A7D1-080A0D090EF4}"/>
+    <hyperlink ref="E9" r:id="rId24" location="CASCON2" display="https://cascon.ca/program/ - CASCON2" xr:uid="{AEF291A1-B334-9149-ADB6-A08474B1EE6E}"/>
+    <hyperlink ref="H5" r:id="rId25" location="CASCON3" display="https://cascon.ca/program/ - CASCON3" xr:uid="{4F746670-2124-0243-A890-EFFB2DDAB8C2}"/>
+    <hyperlink ref="H7" r:id="rId26" location="CASCON4" display="https://cascon.ca/program/ - CASCON4" xr:uid="{86AD4F9A-9827-9249-915A-DC0C0A9E74C8}"/>
+    <hyperlink ref="H9" r:id="rId27" location="CASCON5" display="https://cascon.ca/program/ - CASCON5" xr:uid="{35B56934-3EE5-3047-8511-B40F7A01AFAE}"/>
+    <hyperlink ref="N5" r:id="rId28" location="CASCON6" display="https://cascon.ca/program/ - CASCON6" xr:uid="{637AB7B5-AE20-E24E-95EC-9FCA93947DB0}"/>
+    <hyperlink ref="N7" r:id="rId29" location="CASCON7" display="https://cascon.ca/program/ - CASCON7" xr:uid="{E8A68215-B911-D14D-BB9A-EA6A152D4829}"/>
+    <hyperlink ref="N9" r:id="rId30" location="CASCON8" display="https://cascon.ca/program/ - CASCON8" xr:uid="{EB0DAB3C-289F-FD4C-A871-C58B0ABBA63C}"/>
+    <hyperlink ref="E5" r:id="rId31" display="https://sites.google.com/view/cypress2024/" xr:uid="{F8B4BFBE-7F83-F14D-8F0D-63AEF530B43F}"/>
+    <hyperlink ref="Q9" r:id="rId32" location="NatLang" display="https://cascon.ca/workshops/ - NatLang" xr:uid="{43DF3043-FF6A-A24C-AACE-26632CD05EDF}"/>
+    <hyperlink ref="G11:L11" r:id="rId33" display="CASCON Poster Presentations and Reception" xr:uid="{3AA7171D-8394-0E42-8AE6-6B2708A831E7}"/>
+    <hyperlink ref="K5" r:id="rId34" display="https://users.encs.concordia.ca/~abdelw/oxai2024/" xr:uid="{C8C347A6-13E7-1A41-8F1A-5D13673D45C1}"/>
+    <hyperlink ref="K7" r:id="rId35" display="https://users.encs.concordia.ca/~abdelw/oxai2024/" xr:uid="{615E4B2C-FBBC-0D42-AA28-2007C05D0121}"/>
+    <hyperlink ref="K9" r:id="rId36" display="https://users.encs.concordia.ca/~abdelw/oxai2024/" xr:uid="{0A614FF8-22BB-1C4E-9EA1-A999102C1302}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>